<commit_message>
se pueden generar ambas gráficas y reportes en excel acumulativo. Se requiere de un mayor alcance para poder definir a los tipos de cliente de manera correcta
</commit_message>
<xml_diff>
--- a/archivos_importantes/Instalacion Totalizadores V1.xlsx
+++ b/archivos_importantes/Instalacion Totalizadores V1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msolis\OneDrive - TECH INDUSTRIAS GLOBALES S.R.L\Documentos\ENEL G\CAMPAÑA\8.TOTALIZADORES\ENTREGABLES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvalladares\Downloads\aplicativos_jordan\aplicativo_medidores_totalizadores_enel\archivos_importantes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE48C53-804C-4E0D-8BC0-FE12AFEE4EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284DAAEC-1547-4D0C-9368-C7F620AE4847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instalados acumulados" sheetId="1" state="hidden" r:id="rId1"/>
@@ -2761,13 +2761,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>218190</xdr:colOff>
+      <xdr:colOff>227715</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>171143</xdr:rowOff>
     </xdr:to>
@@ -2792,7 +2792,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2476500"/>
+          <a:off x="9525" y="2476500"/>
           <a:ext cx="7076190" cy="2457143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12415,13 +12415,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14AD160B-C818-4F49-93FE-D73AB2FB388D}">
-  <dimension ref="A1:AS120"/>
+  <dimension ref="A1:AS121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="F109" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E109" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G111" sqref="G111"/>
+      <selection pane="bottomRight" activeCell="I125" sqref="I125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12430,30 +12430,30 @@
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="4"/>
     <col min="4" max="4" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="4" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="4" customWidth="1"/>
     <col min="7" max="7" width="6.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" style="163" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="14" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="14" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" style="4" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" style="4" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" style="4" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="163" customWidth="1"/>
+    <col min="10" max="10" width="11" style="14" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" style="4" customWidth="1"/>
     <col min="15" max="15" width="20.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" style="4" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="8.7109375" style="14" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="12.5703125" style="4" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="11.140625" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="22" max="25" width="9.140625" style="15" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="27" max="30" width="9.140625" style="14" hidden="1" customWidth="1"/>
-    <col min="31" max="42" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="13.85546875" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="20.42578125" style="14" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="17.140625" style="14" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" style="14" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" style="4" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" customWidth="1"/>
+    <col min="22" max="25" width="9.140625" style="15" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" customWidth="1"/>
+    <col min="27" max="30" width="9.140625" style="14" customWidth="1"/>
+    <col min="31" max="42" width="9.140625" customWidth="1"/>
+    <col min="43" max="43" width="13.85546875" customWidth="1"/>
+    <col min="44" max="44" width="20.42578125" style="14" customWidth="1"/>
+    <col min="45" max="45" width="17.140625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:45" x14ac:dyDescent="0.25">
@@ -27363,6 +27363,34 @@
       <c r="AR120" s="90"/>
       <c r="AS120" s="90"/>
     </row>
+    <row r="121" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="B121" s="163"/>
+      <c r="C121" s="14"/>
+      <c r="D121" s="14"/>
+      <c r="I121" s="4"/>
+      <c r="K121" s="4"/>
+      <c r="L121"/>
+      <c r="M121"/>
+      <c r="N121"/>
+      <c r="O121" s="15"/>
+      <c r="P121" s="15"/>
+      <c r="Q121" s="15"/>
+      <c r="R121" s="15"/>
+      <c r="T121" s="14"/>
+      <c r="U121" s="14"/>
+      <c r="V121" s="14"/>
+      <c r="W121" s="14"/>
+      <c r="X121"/>
+      <c r="Y121"/>
+      <c r="AA121"/>
+      <c r="AB121"/>
+      <c r="AC121"/>
+      <c r="AD121"/>
+      <c r="AK121" s="14"/>
+      <c r="AL121" s="14"/>
+      <c r="AR121"/>
+      <c r="AS121"/>
+    </row>
   </sheetData>
   <autoFilter ref="C3:AS88" xr:uid="{14AD160B-C818-4F49-93FE-D73AB2FB388D}"/>
   <mergeCells count="8">
@@ -27382,7 +27410,7 @@
   <conditionalFormatting sqref="C1:C3">
     <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C1:C120 C122:C1048576">
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:C58">
@@ -27400,8 +27428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C711C5-A8C4-46AE-850A-0FC4B97C5FE2}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27534,15 +27562,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010099DA07A05F46024DBD6ACE9246AE17EB" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d389e1dc43977af05cf769669adbd04">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a5a43ca3-cb99-40c2-b67f-57c005bf7e57" xmlns:ns4="9f9f63e2-1e61-45ce-936a-d9bfa596ebae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53e8d6d0b6a21e72e6b370845e9c8563" ns3:_="" ns4:_="">
     <xsd:import namespace="a5a43ca3-cb99-40c2-b67f-57c005bf7e57"/>
@@ -27795,6 +27814,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -27804,14 +27832,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB43897-570A-47EA-9E26-F902C6BA0B1F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF46C923-0D03-4E6C-B3FE-B6D9C7910C4B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27830,6 +27850,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB43897-570A-47EA-9E26-F902C6BA0B1F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2BB2BFD-DF6B-43BB-BDEE-75A60BC40B05}">
   <ds:schemaRefs>

</xml_diff>